<commit_message>
Change conceptual and requirements
</commit_message>
<xml_diff>
--- a/report/requirements/LevantamentoRequisitos.xlsx
+++ b/report/requirements/LevantamentoRequisitos.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\githubUni\BD\report\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Documents\GitHub\BD\report\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC6136D-84FD-4FFC-8CE7-907C25223BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28B98F3-1999-4B33-93A7-89A7947FB618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{921132CD-A3A8-F74A-9E0F-4C9A16FC001E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{921132CD-A3A8-F74A-9E0F-4C9A16FC001E}"/>
   </bookViews>
   <sheets>
     <sheet name="DocumentoGeral" sheetId="1" r:id="rId1"/>
     <sheet name="Requisitos_Descricao" sheetId="2" r:id="rId2"/>
-    <sheet name="Requisitos_Manipulação" sheetId="3" r:id="rId3"/>
+    <sheet name="Requisitos_Exploração" sheetId="3" r:id="rId3"/>
     <sheet name="Requisitos_Controlo" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="97">
   <si>
     <t>Processo de Desenvolvimento do Sistema de Bases de Dados</t>
   </si>
@@ -140,125 +140,9 @@
     <t>RD08</t>
   </si>
   <si>
-    <t>RM01</t>
-  </si>
-  <si>
-    <t>RM02</t>
-  </si>
-  <si>
-    <t>RM03</t>
-  </si>
-  <si>
-    <t>RM04</t>
-  </si>
-  <si>
-    <t>RM05</t>
-  </si>
-  <si>
-    <t>RM06</t>
-  </si>
-  <si>
-    <t>RM07</t>
-  </si>
-  <si>
-    <t>RM08</t>
-  </si>
-  <si>
-    <t>RM09</t>
-  </si>
-  <si>
-    <t>RM10</t>
-  </si>
-  <si>
-    <t>RM11</t>
-  </si>
-  <si>
-    <t>RM12</t>
-  </si>
-  <si>
-    <t>RM13</t>
-  </si>
-  <si>
-    <t>A customer record must contain a unique identifier (number) and optionally fill in the taxpayer number.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A customer's address contains a unique identifier, postal code and city
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Each employee has a unique identifier, a contact with a unique identifier and also a manager (identified by his unique code). Optionally a salary
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A supplier has a mandatory VAT number which will be its unique identifier
-</t>
-  </si>
-  <si>
-    <t>Each item has a unique identifier a name, a purchase price, a sale price and stock, optionally it has a description of the item (size, weight, color, etc..) and the category it belongs to by its identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A category is identified by a key, the name of the category itself, a mandatory tax rate and an optional description of the category.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For a sale to take place, the system must know the customer's number, the employee who processed the sale, the contact of each one, all of this identified by their unique key, status (Done, Pending, Waiting, Error), date of order, date the order was last updated and, if applicable, the price for shipping the order
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organization of the business model;
-</t>
-  </si>
-  <si>
-    <t>Product quality control;</t>
-  </si>
-  <si>
-    <t>Stock control;</t>
-  </si>
-  <si>
-    <t>Control of suppliers (purchase price, product quality, etc.);</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Management of store accounts (tax rate, shipping rate, sales, profits, etc);
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Customer customization, knowing their tastes through past purchases (profiling);
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Establishment of personalized customer discounts.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quality control of orders, namely with regard to shipping time;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indication of the status of the order, allowing the customer to know where he is in the shipping process;
-</t>
-  </si>
-  <si>
-    <t>Knowledge of the products sold, so that it is possible to estimate with more/less output;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knowledge of customer feedback;
-</t>
-  </si>
-  <si>
-    <t>Improve the store's service quality;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comparison between different carriers, in order to choose the most efficient one (time vs. price);
-</t>
-  </si>
-  <si>
     <t>Database System Development Process</t>
   </si>
   <si>
-    <t>Handling Requirements Document</t>
-  </si>
-  <si>
     <t>October 2022</t>
   </si>
   <si>
@@ -295,43 +179,154 @@
     <t>Control Requirements Document</t>
   </si>
   <si>
-    <t xml:space="preserve">Each customer places a certain number of orders and each order has only one associated customer.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An order has several items (amount attribute tells us the number of items in the order) and the same item can be present in several orders.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An item can have multiple suppliers and the same supplier can supply multiple items.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A supplier has only one contact (e-mail, mobile phone, name) and this contact is unique, that is, it is only present for that supplier.
-</t>
-  </si>
-  <si>
-    <t>A customer has only one contact (e-mail, mobile phone, name) and this contact is unique, that is, it is only present for that customer.</t>
-  </si>
-  <si>
-    <t>An employee has only one contact (e-mail, cell phone, name) and this contact is unique, that is, it is only present for that employee.</t>
-  </si>
-  <si>
-    <t>A customer can have several addresses and the same address can be associated with several customers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An order has only one associated employee, however, the same employee can have several orders associated with it.
-</t>
-  </si>
-  <si>
-    <t>An item has a certain type associated with it. The same type can cover several items.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A manager can have several employees, however, an employee only has one manager.
-</t>
-  </si>
-  <si>
-    <t>A contact is identified by a code, also having the name, mobile phone number and email</t>
+    <t>A caracterização de um cliente na base de dados deve incluir um identificador único e opcionalmente um número fiscal associado a ele. Deve também, obrigatoriamente, incluir um contacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uma morada deve conter um identificador único, o nome da rua, o código postal e a cidade de residência. </t>
+  </si>
+  <si>
+    <t>Um contacto deve conter um identificador único, o nome da pessoa/instituição em questão, o email e o número de telemóvel.</t>
+  </si>
+  <si>
+    <t>Cada encomenda deve ter um identificador único, um status, um preço de envio da encomenda opcional, uma data de entrada da encomenda e uma data com a última alteração feita na encomenda. Deve ainda ter um identificador para o funcionário responsável pela encomenda, e um identificador para o cliente que fez a encomenda.</t>
+  </si>
+  <si>
+    <t>A entidade empregado deve ter um identificador único, um campo que identifique o manager, um campo que identifique o salário do empregado e um campo que contenha um identificador único para o contacto do  empregado.</t>
+  </si>
+  <si>
+    <t>Um fornecedor deve conter o seu NIF como identificador único e um contacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uma categoria deve conter um indentificador único bem como o seu nome, uma descrição e a taxa associada a essa categoria </t>
+  </si>
+  <si>
+    <t>Um item contém um identificador único, o seu nome, uma descrição do item,  um campo que indica o número de stock desse item, o seu preço de venda e de compra e ainda a categoria a que pertence</t>
+  </si>
+  <si>
+    <t>Requisitos de Exploração</t>
+  </si>
+  <si>
+    <t>RD09</t>
+  </si>
+  <si>
+    <t>Um cliente apenas pode ter um contacto</t>
+  </si>
+  <si>
+    <t>Um fornecedor apenas pode ter um contacto</t>
+  </si>
+  <si>
+    <t>Um empregado apenas pode ter um contacto</t>
+  </si>
+  <si>
+    <t>Um cliente pode ter várias moradas e várias moradas podem estar associadas a vários clientes</t>
+  </si>
+  <si>
+    <t>Um cliente pode fazer várias encomendas mas uma encomenda está associada apenas a um cliente.</t>
+  </si>
+  <si>
+    <t>Uma encomenda pode ter vários items e vários items podem estar presentes em várias encomendas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uma encomenda pode estar associada apenas a um empregado mas um empregado pode estar associado a várias encomendas </t>
+  </si>
+  <si>
+    <t>Um item pode ser fornecido por vários fornecedores e um fornecedor pode fornecer vários items</t>
+  </si>
+  <si>
+    <t>Um categoria incorpora vários items no entanto um item apenas pertence a uma categoria</t>
+  </si>
+  <si>
+    <t>Uma encomenda contém uma certa quantidade de um item.</t>
+  </si>
+  <si>
+    <t>Deve ser possível alterar o estado do pedido e dar update à última operação efetuada.</t>
+  </si>
+  <si>
+    <t>Deve ser possível inserir novos contactos</t>
+  </si>
+  <si>
+    <t>Deve ser possível alterar informação de um contacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deve ser possível apagar um contacto </t>
+  </si>
+  <si>
+    <t>Deve ser possível listar todas as encomendas realizadas num certo dia do mês</t>
+  </si>
+  <si>
+    <t>Deve ser possível listar encomendas num dado estado duma dada categoria de items</t>
+  </si>
+  <si>
+    <t>Deve ser possível listar todas as encomendas com a morada de entrega do cliente correspondente à encomenda</t>
+  </si>
+  <si>
+    <t>Deve ser possível listar todas as encomendas atríbuidas a um dado funcionário</t>
+  </si>
+  <si>
+    <t>Deve ser possível listar todas as encomendas feitas por um cliente</t>
+  </si>
+  <si>
+    <t>Deve ser possível fazer um top X de clientes, em que o valor de X fica ao encargo do utilizador</t>
+  </si>
+  <si>
+    <t>Deve ser possível saber quantos e quais items compramos a um certo fornecedor</t>
+  </si>
+  <si>
+    <t>Deve ser possível listar o stock de items disponível</t>
+  </si>
+  <si>
+    <t>Deve ser possível ordenar os items por número de stock</t>
+  </si>
+  <si>
+    <t>Deve ser possível ordenar as categorias por nome</t>
+  </si>
+  <si>
+    <t>Deve ser possível ordenar os funcionários por ordem decrescente de salário</t>
+  </si>
+  <si>
+    <t>RE01</t>
+  </si>
+  <si>
+    <t>RE02</t>
+  </si>
+  <si>
+    <t>RE03</t>
+  </si>
+  <si>
+    <t>RE04</t>
+  </si>
+  <si>
+    <t>RE05</t>
+  </si>
+  <si>
+    <t>RE06</t>
+  </si>
+  <si>
+    <t>RE07</t>
+  </si>
+  <si>
+    <t>RE08</t>
+  </si>
+  <si>
+    <t>RE09</t>
+  </si>
+  <si>
+    <t>RE10</t>
+  </si>
+  <si>
+    <t>RE11</t>
+  </si>
+  <si>
+    <t>RE12</t>
+  </si>
+  <si>
+    <t>RE13</t>
+  </si>
+  <si>
+    <t>RE14</t>
+  </si>
+  <si>
+    <t>RE15</t>
   </si>
 </sst>
 </file>
@@ -777,7 +772,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -854,14 +849,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33507E5-9B7D-474E-9F9F-319052DA68F0}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="69" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="60.19921875" customWidth="1"/>
     <col min="4" max="4" width="19.69921875" customWidth="1"/>
+    <col min="7" max="7" width="73.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="91.8" x14ac:dyDescent="1.65">
@@ -872,20 +868,20 @@
     </row>
     <row r="2" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
@@ -893,13 +889,13 @@
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="11" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -907,22 +903,22 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
@@ -933,9 +929,9 @@
       <c r="D10" s="10"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
@@ -946,7 +942,7 @@
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
@@ -954,72 +950,72 @@
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" ht="78" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1027,7 +1023,9 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1092,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258A5496-A7EE-504A-AA66-0C7E29D70A04}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1112,20 +1110,20 @@
     </row>
     <row r="2" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
@@ -1133,13 +1131,13 @@
     </row>
     <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="12" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1147,27 +1145,27 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -1175,10 +1173,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -1186,10 +1184,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -1197,32 +1195,32 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -1230,10 +1228,10 @@
     </row>
     <row r="16" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -1241,32 +1239,32 @@
     </row>
     <row r="17" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -1274,21 +1272,21 @@
     </row>
     <row r="20" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
@@ -1296,25 +1294,33 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="C23" s="9"/>
+      <c r="A23" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="C24" s="9"/>
+      <c r="A24" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
@@ -1332,6 +1338,9 @@
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1347,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE65A420-5C1D-DC4C-80EF-F93CF3287211}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A4" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1365,20 +1374,20 @@
     </row>
     <row r="2" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
@@ -1386,13 +1395,13 @@
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="12" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1400,80 +1409,80 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="9" t="s">
-        <v>81</v>
+      <c r="C10" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="8" t="s">
-        <v>82</v>
+      <c r="C11" t="s">
+        <v>58</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1486,7 +1495,7 @@
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1499,20 +1508,20 @@
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -1525,20 +1534,20 @@
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1548,7 +1557,6 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>

</xml_diff>

<commit_message>
GG well played :100:
</commit_message>
<xml_diff>
--- a/report/requirements/LevantamentoRequisitos.xlsx
+++ b/report/requirements/LevantamentoRequisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Documents\GitHub\BD\report\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28B98F3-1999-4B33-93A7-89A7947FB618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F87A544-7CE7-4C3B-A593-80F1BD8EE4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{921132CD-A3A8-F74A-9E0F-4C9A16FC001E}"/>
   </bookViews>
@@ -850,12 +850,13 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="60.19921875" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="67.09765625" customWidth="1"/>
     <col min="4" max="4" width="19.69921875" customWidth="1"/>
     <col min="7" max="7" width="73.8984375" customWidth="1"/>
   </cols>
@@ -1093,7 +1094,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1357,12 +1358,13 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="45.5" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" customWidth="1"/>
+    <col min="3" max="3" width="53.3984375" customWidth="1"/>
     <col min="4" max="4" width="23.19921875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Update last presentation :anchor:
</commit_message>
<xml_diff>
--- a/report/requirements/LevantamentoRequisitos.xlsx
+++ b/report/requirements/LevantamentoRequisitos.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Documents\GitHub\BD\report\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F87A544-7CE7-4C3B-A593-80F1BD8EE4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DE681F-BD19-40AE-86CC-74A8391CFDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{921132CD-A3A8-F74A-9E0F-4C9A16FC001E}"/>
   </bookViews>
   <sheets>
     <sheet name="DocumentoGeral" sheetId="1" r:id="rId1"/>
     <sheet name="Requisitos_Descricao" sheetId="2" r:id="rId2"/>
-    <sheet name="Requisitos_Exploração" sheetId="3" r:id="rId3"/>
-    <sheet name="Requisitos_Controlo" sheetId="4" r:id="rId4"/>
+    <sheet name="Folha2" sheetId="6" r:id="rId3"/>
+    <sheet name="Requisitos_Exploração" sheetId="3" r:id="rId4"/>
+    <sheet name="Folha1" sheetId="5" r:id="rId5"/>
+    <sheet name="Requisitos_Controlo" sheetId="4" r:id="rId6"/>
+    <sheet name="Folha3" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="130">
   <si>
     <t>Processo de Desenvolvimento do Sistema de Bases de Dados</t>
   </si>
@@ -327,6 +330,105 @@
   </si>
   <si>
     <t>RE15</t>
+  </si>
+  <si>
+    <t>It must be possible to change the status of the order and update the last operation performed.</t>
+  </si>
+  <si>
+    <t>It must be possible to insert new contacts</t>
+  </si>
+  <si>
+    <t>It must be possible to change contact information</t>
+  </si>
+  <si>
+    <t>It must be possible to delete a contact</t>
+  </si>
+  <si>
+    <t>It should be possible to list all orders placed on a certain day of the month</t>
+  </si>
+  <si>
+    <t>It must be possible to list orders in a given status of a given category of items</t>
+  </si>
+  <si>
+    <t>It must be possible to list all orders with the delivery address of the customer corresponding to the order</t>
+  </si>
+  <si>
+    <t>It must be possible to list all orders assigned to a given employee</t>
+  </si>
+  <si>
+    <t>It should be possible to list all orders placed by a customer</t>
+  </si>
+  <si>
+    <t>It must be possible to make a top X of customers, where the value of X is up to the user</t>
+  </si>
+  <si>
+    <t>It must be possible to know how many and which items we buy from a certain supplier</t>
+  </si>
+  <si>
+    <t>It must be possible to list the stock of available items</t>
+  </si>
+  <si>
+    <t>It should be possible to sort items by stock number</t>
+  </si>
+  <si>
+    <t>It should be possible to sort categories by name</t>
+  </si>
+  <si>
+    <t>It should be possible to sort employees in descending order of salary</t>
+  </si>
+  <si>
+    <t>The characterization of a customer in the database must include a unique identifier and optionally an associated tax number. It must also, obligatorily, include a contact</t>
+  </si>
+  <si>
+    <t>An address must contain a unique identifier, street name, postal code and city of residence.</t>
+  </si>
+  <si>
+    <t>A contact must contain a unique identifier, the name of the person/institution in question, email and mobile phone number.</t>
+  </si>
+  <si>
+    <t>Each order must have a unique identifier, a status, an optional order shipping price, an order entry date, and a date with the last change made to the order. It must also have an identifier for the employee responsible for the order, and an identifier for the customer who placed the order.</t>
+  </si>
+  <si>
+    <t>The employee entity must have a unique identifier, a field that identifies the manager, a field that identifies the employee's salary, and a field that contains a unique identifier for the employee's contact.</t>
+  </si>
+  <si>
+    <t>A supplier must contain his NIF as a unique identifier and a contact</t>
+  </si>
+  <si>
+    <t>A category must contain a unique identifier as well as its name, a description and the tax associated with that category.</t>
+  </si>
+  <si>
+    <t>An item contains a unique identifier, its name, a description of the item, a field that indicates the stock number of that item, its sale and purchase price and also the category to which it belongs</t>
+  </si>
+  <si>
+    <t>A customer can only have one contact</t>
+  </si>
+  <si>
+    <t>A supplier can only have one contact</t>
+  </si>
+  <si>
+    <t>An employee can only have one contact</t>
+  </si>
+  <si>
+    <t>A customer can have multiple addresses and multiple addresses can be associated with multiple customers</t>
+  </si>
+  <si>
+    <t>A customer can place several orders, but an order is associated with only one customer.</t>
+  </si>
+  <si>
+    <t>An order can have several items and several items can be present in several orders</t>
+  </si>
+  <si>
+    <t>An order can only be associated with one employee, but an employee can be associated with multiple orders.</t>
+  </si>
+  <si>
+    <t>One item can be supplied by multiple suppliers and one supplier can supply multiple items.</t>
+  </si>
+  <si>
+    <t>A category incorporates several items, however an item only belongs to one category</t>
+  </si>
+  <si>
+    <t>An order contains a certain quantity of an item.</t>
   </si>
 </sst>
 </file>
@@ -849,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33507E5-9B7D-474E-9F9F-319052DA68F0}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1090,11 +1192,253 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D88BBD-7016-47DD-9C77-84AE31BFC3B8}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="77.8984375" customWidth="1"/>
+    <col min="4" max="4" width="19.69921875" customWidth="1"/>
+    <col min="7" max="7" width="73.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="91.8" x14ac:dyDescent="1.65">
+      <c r="A1" s="4"/>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="A7" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258A5496-A7EE-504A-AA66-0C7E29D70A04}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1353,12 +1697,274 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FFBBBA8-27DE-4323-8F71-FEB5A3E51CB3}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="67.69921875" customWidth="1"/>
+    <col min="4" max="4" width="20.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="91.8" x14ac:dyDescent="1.65">
+      <c r="A1" s="4"/>
+      <c r="E1" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+      <c r="A7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE65A420-5C1D-DC4C-80EF-F93CF3287211}">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1491,7 +2097,7 @@
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>28</v>
       </c>
@@ -1517,7 +2123,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>30</v>
       </c>
@@ -1543,7 +2149,7 @@
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>32</v>
       </c>
@@ -1571,4 +2177,223 @@
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5A8571-B210-4D3F-B0A1-4F4480556FB5}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C19" sqref="C10:C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.59765625" customWidth="1"/>
+    <col min="3" max="3" width="53.3984375" customWidth="1"/>
+    <col min="4" max="4" width="23.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="91.8" x14ac:dyDescent="1.65">
+      <c r="A1" s="4"/>
+      <c r="F1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="A7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>